<commit_message>
changes made for coverage
</commit_message>
<xml_diff>
--- a/validation_report.xlsx
+++ b/validation_report.xlsx
@@ -1,15 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Missing Sections" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Extra Sections" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,89 +436,87 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Total ToC Sections</t>
+          <t>Metadata Status</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Total Parsed Sections</t>
+          <t>Total ToC Entries</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Missing Sections</t>
+          <t>Sections Parsed</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Extra Sections</t>
+          <t>TOC Covered Pages</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Pages with Text</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Page Coverage (%)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Content Coverage (%)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>TOC Coverage (%)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>JSONL Records</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Inheritance Detected</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>81</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Valid</t>
+        </is>
       </c>
       <c r="B2" t="n">
-        <v>81</v>
+        <v>1005</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1021</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Missing Sections</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Extra Sections</t>
-        </is>
+        <v>1031</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1047</v>
+      </c>
+      <c r="F2" t="n">
+        <v>100</v>
+      </c>
+      <c r="G2" t="n">
+        <v>97.52</v>
+      </c>
+      <c r="H2" t="n">
+        <v>98.47</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1021</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved Modularity and OOP
</commit_message>
<xml_diff>
--- a/validation_report.xlsx
+++ b/validation_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,14 +451,14 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Pages with Text</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>TOC Covered Pages</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Pages with Text</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Page Coverage (%)</t>
@@ -466,22 +466,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Content Coverage (%)</t>
+          <t>TOC Coverage (%)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>TOC Coverage (%)</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>JSONL Records</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Inheritance Detected</t>
+          <t>Section Coverage (%)</t>
         </is>
       </c>
     </row>
@@ -498,25 +488,19 @@
         <v>1021</v>
       </c>
       <c r="D2" t="n">
+        <v>1047</v>
+      </c>
+      <c r="E2" t="n">
         <v>1031</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1047</v>
       </c>
       <c r="F2" t="n">
         <v>100</v>
       </c>
       <c r="G2" t="n">
+        <v>98.47</v>
+      </c>
+      <c r="H2" t="n">
         <v>97.52</v>
-      </c>
-      <c r="H2" t="n">
-        <v>98.47</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1021</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes made for content extraction and Quality
</commit_message>
<xml_diff>
--- a/validation_report.xlsx
+++ b/validation_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,16 +464,6 @@
           <t>Page Coverage (%)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>TOC Coverage (%)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Section Coverage (%)</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -482,25 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1005</v>
+        <v>922</v>
       </c>
       <c r="C2" t="n">
-        <v>1021</v>
+        <v>3635</v>
       </c>
       <c r="D2" t="n">
         <v>1047</v>
       </c>
       <c r="E2" t="n">
-        <v>1031</v>
+        <v>1014</v>
       </c>
       <c r="F2" t="n">
         <v>100</v>
-      </c>
-      <c r="G2" t="n">
-        <v>98.47</v>
-      </c>
-      <c r="H2" t="n">
-        <v>97.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>